<commit_message>
Improve canister behavior calculations
- Use volumetric flow rate instead of mass flow across orifice when
  determining canister fill time
- See how ambient conditions affect fill time
- Change canister max fill ratio to safety margin
</commit_message>
<xml_diff>
--- a/engr/CanisterDesign.xlsx
+++ b/engr/CanisterDesign.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\WSU SMART REA\design.git\engr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="16980" windowHeight="8160" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="16980" windowHeight="8160" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Canisters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -18,74 +23,270 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Patrick O'Keeffe</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1976 Standard Atmosphere</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Orifice flow under choked conditions at 70ºF, 14.7psia (mnfctr STP).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Canister final pressure must be less than 52.8% of barometric pressure to maintain choked flow; specify additional safety margin. Example: 10% = final pressure is 42.8% of barometric.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction of standard deviation of vertical wind speed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Duration of time spent sampling each day. This affects canister fill time and power consumption.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assuming vertical wind speed is normally distributed. (Quality of assumption unknown)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Assuming equal time sampling into each canister. (Fairly realistic)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Sampling Flow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+  <si>
+    <t>Canister volume</t>
+  </si>
+  <si>
+    <t>liters</t>
+  </si>
+  <si>
+    <t>Deadband</t>
+  </si>
+  <si>
+    <t>Fraction of time in deadband</t>
+  </si>
+  <si>
+    <t>Fraction of time per canister</t>
+  </si>
+  <si>
+    <t>(multiplier)</t>
+  </si>
+  <si>
+    <t>Canister full safety margin</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Sampling hours per day</t>
+  </si>
+  <si>
+    <t>Canister fill time</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Orifice flow @ STP</t>
   </si>
   <si>
     <t>sccm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>**Smallest critical orifice I can find</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Canister Volume</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Canister Fill Fraction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Deadband </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>**Multiplier of Std Dev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fraction of Time Excluded</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>**Assumes w is normally distributed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fraction of Time per Canister</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>**Must be &lt; 50% to maintain critical flow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cm3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hours of Sampling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Days of Sampling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Barometric pressure</t>
+  </si>
+  <si>
+    <t>Ambient temp</t>
+  </si>
+  <si>
+    <t>ºF</t>
+  </si>
+  <si>
+    <t>Actual orifice flow</t>
+  </si>
+  <si>
+    <t>cc/min</t>
+  </si>
+  <si>
+    <t>User Input</t>
+  </si>
+  <si>
+    <t>Derived Values</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>mbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sea level </t>
+  </si>
+  <si>
+    <t>Pullman (2550')</t>
+  </si>
+  <si>
+    <t>Denver (5280')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -94,13 +295,61 @@
       <sz val="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,21 +361,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -449,110 +727,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1013</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>923</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1">
+        <v>834</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>33000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.85</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <f>ERF(B6/SQRT(2))</f>
-        <v>0.60467491375461524</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <f>(1-B8)/2</f>
-        <v>0.19766254312269238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3">
-        <f>B3*B4/B1/B9/60</f>
-        <v>185.5013402509299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
-        <f>B11/24</f>
-        <v>7.7292225104554122</v>
+      <c r="B12" s="4">
+        <v>923</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3">
+        <f>B11*(14.7/(B12/68.947573))*((B13+460)/530)</f>
+        <v>6.4020229530019002</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
+        <f>ERF(B16/SQRT(2))</f>
+        <v>0.60467491375461524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <f>(1-B21)/2</f>
+        <v>0.19766254312269238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2">
+        <f>B14*(0.528-B15)*1000/(B20*B22*60*B17)</f>
+        <v>7.7509263683374092</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>